<commit_message>
J-Esquema Mouredev y cambios Prototypes
</commit_message>
<xml_diff>
--- a/Apuntes/LanguajePrototype/06-Logica Booleana/Adjuntos/LogicaBooleana.xlsx
+++ b/Apuntes/LanguajePrototype/06-Logica Booleana/Adjuntos/LogicaBooleana.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar Ardevol\Documents\VSC\Proyectos GitHub\Teoria\Apuntes\LanguajePrototype\06-Logica Booleana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar Ardevol\Documents\VSC\Proyectos GitHub\Teoria\Apuntes\LanguajePrototype\06-Logica Booleana\Adjuntos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0994CCB8-8302-474C-9EBE-A103889510D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C20BD23-951E-422F-9B33-F3C9D04EFAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Operadores de igualdad</t>
   </si>
@@ -186,6 +186,39 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Formulas anidadas</t>
+  </si>
+  <si>
+    <t>0=Falso</t>
+  </si>
+  <si>
+    <t>1=Falso</t>
+  </si>
+  <si>
+    <t>Truthy/Falsy</t>
+  </si>
+  <si>
+    <t>Operadores logicos</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>True si se cumplen todas las condiciones</t>
+  </si>
+  <si>
+    <t>True si se cumplen alguna de las condiciones</t>
+  </si>
+  <si>
+    <t>Devuelve el contrario de el resultado</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
   </si>
 </sst>
 </file>
@@ -307,13 +340,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -325,6 +354,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,16 +639,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
     <col min="12" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -622,228 +656,302 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="str" cm="1">
+        <f t="array" ref="B2">{"a=b"}</f>
+        <v>a=b</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <f>E2=F2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2">{"="}</f>
-        <v>=</v>
-      </c>
-      <c r="C2" t="b">
-        <f>E2=F2</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="N2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="B3" s="2" t="str" cm="1">
+        <f t="array" ref="B3">{"a&gt;b"}</f>
+        <v>a&gt;b</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <f>E2&gt;F2</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="str" cm="1">
-        <f t="array" ref="B3">{"="}</f>
-        <v>=</v>
-      </c>
-      <c r="C3" t="b">
-        <f>E2&gt;F2</f>
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="B4" s="2" t="str" cm="1">
+        <f t="array" ref="B4">{"a&lt;b"}</f>
+        <v>a&lt;b</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <f>E2&lt;F2</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <f>I4*J4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="12" t="b">
+        <f t="shared" ref="L4:L5" si="0">AND(I4,J4)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="12" t="b">
+        <f t="shared" ref="M4:M5" si="1">OR(I4:J4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="b">
+        <f>NOT(L4)</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="b">
+        <f>NOT(M4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="str" cm="1">
+        <f t="array" ref="B5">{"a&gt;=b"}</f>
+        <v>a&gt;=b</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <f>E2&gt;=F2</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <f>I5*J5</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N5" s="2" t="b">
+        <f t="shared" ref="N5:N6" si="2">NOT(L5)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="b">
+        <f t="shared" ref="O5:O6" si="3">NOT(M5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="str" cm="1">
+        <f t="array" ref="B6">{"a&lt;=b"}</f>
+        <v>a&lt;=b</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <f>E2&lt;=F2</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <f>I6*J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="13" t="b">
+        <f>AND(I6,J6)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="13" t="b">
+        <f>OR(I6:J6)</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="2" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="str" cm="1">
+        <f t="array" ref="B7">{"a&lt;&gt;b"}</f>
+        <v>a&lt;&gt;b</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <f>E2&lt;&gt;F2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="str" cm="1">
+        <f t="array" ref="B8">{"a==b"}</f>
+        <v>a==b</v>
+      </c>
+      <c r="C8" s="5" t="b">
+        <f>TYPE(E2)=TYPE(G2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="str" cm="1">
-        <f t="array" ref="B4">{"="}</f>
-        <v>=</v>
-      </c>
-      <c r="C4" t="b">
-        <f>E2&lt;F2</f>
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <f>I4*J4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="b">
-        <f t="shared" ref="L4:L5" si="0">AND(I4,J4)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="b">
-        <f t="shared" ref="M4:M5" si="1">OR(I4:J4)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" t="b">
-        <f>NOT(L4)</f>
-        <v>1</v>
-      </c>
-      <c r="O4" t="b">
-        <f>NOT(M4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="str" cm="1">
-        <f t="array" ref="B5">{"&gt;="}</f>
-        <v>&gt;=</v>
-      </c>
-      <c r="C5" t="b">
-        <f>E2&gt;=F2</f>
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <f>I5*J5</f>
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M5" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N5" t="b">
-        <f t="shared" ref="N5:N6" si="2">NOT(L5)</f>
-        <v>0</v>
-      </c>
-      <c r="O5" t="b">
-        <f t="shared" ref="O5:O6" si="3">NOT(M5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="str" cm="1">
-        <f t="array" ref="B6">{"&lt;="}</f>
-        <v>&lt;=</v>
-      </c>
-      <c r="C6" t="b">
-        <f>E2&lt;=F2</f>
-        <v>1</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <f>I6*J6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="2" t="b">
-        <f>AND(I6,J6)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="2" t="b">
-        <f>OR(I6:J6)</f>
-        <v>1</v>
-      </c>
-      <c r="N6" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O6" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="str" cm="1">
-        <f t="array" ref="B7">{"&lt;&gt;"}</f>
-        <v>&lt;&gt;</v>
-      </c>
-      <c r="C7" t="b">
-        <f>E2&lt;&gt;F2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="str" cm="1">
-        <f t="array" ref="B8">{"=="}</f>
-        <v>==</v>
-      </c>
-      <c r="C8" t="b">
-        <f>TYPE(E2)=TYPE(G2)</f>
+      <c r="B12" s="5" t="b">
+        <f>AND(TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5" t="b">
+        <f>OR(TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="5" t="b">
+        <f>NOT(TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="b">
+        <f>0=FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="b">
+        <f>1=FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -858,10 +966,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFBDA45-F3C8-4B84-B41C-7D91A6D45E8B}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,22 +987,22 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G2" t="s">
@@ -902,24 +1010,24 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="b">
+      <c r="C3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="b">
         <f>B3&gt;=18</f>
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="b">
+      <c r="E3" s="2" t="b">
         <f>B3&gt;=25</f>
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="b">
+      <c r="F3" s="2" t="b">
         <f>AND(E3,NOT(C3))</f>
         <v>0</v>
       </c>
@@ -929,24 +1037,24 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="b">
+      <c r="C4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="b">
         <f t="shared" ref="D4:D6" si="0">B4&gt;=18</f>
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="b">
+      <c r="E4" s="2" t="b">
         <f t="shared" ref="E4:E6" si="1">B4&gt;=25</f>
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="b">
+      <c r="F4" s="2" t="b">
         <f t="shared" ref="F4:F6" si="2">AND(E4,NOT(C4))</f>
         <v>0</v>
       </c>
@@ -956,24 +1064,24 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="b">
+      <c r="C5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="b">
+      <c r="E5" s="2" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="b">
+      <c r="F5" s="2" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -983,24 +1091,24 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="b">
+      <c r="C6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="4" t="b">
+      <c r="E6" s="2" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F6" s="4" t="b">
+      <c r="F6" s="2" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1009,71 +1117,76 @@
         <v>Edad Entrar Disco = FALSO; Problemas Alcohol = FALSO; Edad Alcohol = FALSO;  --&gt;Venta Alcohol = FALSO</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="str">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="str">
         <f>A2</f>
         <v>Persona</v>
       </c>
-      <c r="B9" s="5" t="str">
-        <f t="shared" ref="B9:C9" si="4">B2</f>
+      <c r="B11" s="3" t="str">
+        <f t="shared" ref="B11:C11" si="4">B2</f>
         <v>Edad</v>
       </c>
-      <c r="C9" s="8" t="str">
+      <c r="C11" s="6" t="str">
         <f t="shared" si="4"/>
         <v>Problemas Alcohol</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <f t="shared" ref="A10:C11" si="5">A3</f>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="str">
+        <f>A3</f>
         <v>Jimy</v>
       </c>
-      <c r="B10" s="4">
-        <f t="shared" si="5"/>
+      <c r="B12" s="2">
+        <f>B3</f>
         <v>18</v>
       </c>
-      <c r="C10" s="9" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="7" t="str">
-        <f>IF(AND(B10&gt;=25,NOT(C10)),"Vendemos","NoVendemos")</f>
+      <c r="C12" s="7" t="b">
+        <f>C3</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <f>IF(AND(B12&gt;=25,NOT(C12)),"Vendemos","NoVendemos")</f>
         <v>NoVendemos</v>
       </c>
-      <c r="E10" s="11" t="str">
+      <c r="E12" s="9" t="str">
         <f>_xlfn.LET(
-_xlpm.edadCliente,                 B10,
+_xlpm.edadCliente,                 B12,
 _xlpm.edadAlchohol,              25,
-_xlpm.problemasAlcohol,    C10,
+_xlpm.problemasAlcohol,    C12,
 _xlpm.edadConsumo,           _xlpm.edadCliente &gt;= _xlpm.edadAlchohol,
 _xlpm.puedeBeber,                NOT(_xlpm.problemasAlcohol),
 _xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
@@ -1081,103 +1194,7 @@
 _xlpm.respuesta)</f>
         <v>NoVendemos</v>
       </c>
-      <c r="F10" s="11" t="str">
-        <f>_xlfn.LET(
-_xlpm.edadCliente,                 B10,
-_xlpm.edadAlchohol,             25,
-_xlpm.problemasAlcohol,    C10,
-_xlpm.edadEntrada,                18,
-_xlpm.edadConsumo,            _xlpm.edadCliente &gt;= _xlpm.edadAlchohol,
-_xlpm.puedeBeber,                NOT(_xlpm.problemasAlcohol),
-_xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
-_xlpm.permisoEntrada,          _xlpm.edadCliente &gt;=  _xlpm.edadEntrada,
-_xlpm.respuestaEntrada,       IF(_xlpm.permisoEntrada,"SinAlchohol","NoPasar"),
-_xlpm.respuesta,                      IF(_xlpm.condicionesBeber,"Vendemos",_xlpm.respuestaEntrada),
-_xlpm.respuesta)</f>
-        <v>SinAlchohol</v>
-      </c>
-      <c r="G10" s="4" t="str">
-        <f>IF(
-OR(F10="SinAlchohol",F10="EntradaNormal"),
-"Bienvenido",
-"Lo sentimos no puede pasar")</f>
-        <v>Bienvenido</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>Carol</v>
-      </c>
-      <c r="B11" s="4">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="C11" s="9" t="b">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="D11" s="7" t="str">
-        <f t="shared" ref="D11:D13" si="6">IF(AND(B11&gt;=25,NOT(C11)),"Vendemos","NoVendemos")</f>
-        <v>NoVendemos</v>
-      </c>
-      <c r="E11" s="11" t="str">
-        <f t="shared" ref="E11:E13" si="7">_xlfn.LET(
-_xlpm.edadCliente,                 B11,
-_xlpm.edadAlchohol,              25,
-_xlpm.problemasAlcohol,    C11,
-_xlpm.edadConsumo,           _xlpm.edadCliente &gt;= _xlpm.edadAlchohol,
-_xlpm.puedeBeber,                NOT(_xlpm.problemasAlcohol),
-_xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
-_xlpm.respuesta,                      IF(_xlpm.condicionesBeber,"Vendemos","NoVendemos"),
-_xlpm.respuesta)</f>
-        <v>NoVendemos</v>
-      </c>
-      <c r="F11" s="11" t="str">
-        <f t="shared" ref="F11:F13" si="8">_xlfn.LET(
-_xlpm.edadCliente,                 B11,
-_xlpm.edadAlchohol,             25,
-_xlpm.problemasAlcohol,    C11,
-_xlpm.edadEntrada,                18,
-_xlpm.edadConsumo,            _xlpm.edadCliente &gt;= _xlpm.edadAlchohol,
-_xlpm.puedeBeber,                NOT(_xlpm.problemasAlcohol),
-_xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
-_xlpm.permisoEntrada,          _xlpm.edadCliente &gt;=  _xlpm.edadEntrada,
-_xlpm.respuestaEntrada,       IF(_xlpm.permisoEntrada,"SinAlchohol","NoPasar"),
-_xlpm.respuesta,                      IF(_xlpm.condicionesBeber,"Vendemos",_xlpm.respuestaEntrada),
-_xlpm.respuesta)</f>
-        <v>SinAlchohol</v>
-      </c>
-      <c r="G11" s="4" t="str">
-        <f t="shared" ref="G11:G12" si="9">IF(
-OR(F11="SinAlchohol",F11="EntradaNormal"),
-"Bienvenido",
-"Lo sentimos no puede pasar")</f>
-        <v>Bienvenido</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <f t="shared" ref="A12:C13" si="10">A5</f>
-        <v>Billy</v>
-      </c>
-      <c r="B12" s="4">
-        <f t="shared" si="10"/>
-        <v>25</v>
-      </c>
-      <c r="C12" s="9" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>Vendemos</v>
-      </c>
-      <c r="E12" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>Vendemos</v>
-      </c>
-      <c r="F12" s="11" t="str">
+      <c r="F12" s="9" t="str">
         <f>_xlfn.LET(
 _xlpm.edadCliente,                 B12,
 _xlpm.edadAlchohol,             25,
@@ -1188,43 +1205,139 @@
 _xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
 _xlpm.permisoEntrada,          _xlpm.edadCliente &gt;=  _xlpm.edadEntrada,
 _xlpm.respuestaEntrada,       IF(_xlpm.permisoEntrada,"SinAlchohol","NoPasar"),
+_xlpm.respuesta,                      IF(_xlpm.condicionesBeber,"Vendemos",_xlpm.respuestaEntrada),
+_xlpm.respuesta)</f>
+        <v>SinAlchohol</v>
+      </c>
+      <c r="G12" s="2" t="str">
+        <f>IF(
+OR(F12="SinAlchohol",F12="EntradaNormal"),
+"Bienvenido",
+"Lo sentimos no puede pasar")</f>
+        <v>Bienvenido</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="str">
+        <f>A4</f>
+        <v>Carol</v>
+      </c>
+      <c r="B13" s="2">
+        <f>B4</f>
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="b">
+        <f>C4</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <f t="shared" ref="D13:D15" si="5">IF(AND(B13&gt;=25,NOT(C13)),"Vendemos","NoVendemos")</f>
+        <v>NoVendemos</v>
+      </c>
+      <c r="E13" s="9" t="str">
+        <f t="shared" ref="E13:E15" si="6">_xlfn.LET(
+_xlpm.edadCliente,                 B13,
+_xlpm.edadAlchohol,              25,
+_xlpm.problemasAlcohol,    C13,
+_xlpm.edadConsumo,           _xlpm.edadCliente &gt;= _xlpm.edadAlchohol,
+_xlpm.puedeBeber,                NOT(_xlpm.problemasAlcohol),
+_xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
+_xlpm.respuesta,                      IF(_xlpm.condicionesBeber,"Vendemos","NoVendemos"),
+_xlpm.respuesta)</f>
+        <v>NoVendemos</v>
+      </c>
+      <c r="F13" s="9" t="str">
+        <f t="shared" ref="F13:F15" si="7">_xlfn.LET(
+_xlpm.edadCliente,                 B13,
+_xlpm.edadAlchohol,             25,
+_xlpm.problemasAlcohol,    C13,
+_xlpm.edadEntrada,                18,
+_xlpm.edadConsumo,            _xlpm.edadCliente &gt;= _xlpm.edadAlchohol,
+_xlpm.puedeBeber,                NOT(_xlpm.problemasAlcohol),
+_xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
+_xlpm.permisoEntrada,          _xlpm.edadCliente &gt;=  _xlpm.edadEntrada,
+_xlpm.respuestaEntrada,       IF(_xlpm.permisoEntrada,"SinAlchohol","NoPasar"),
+_xlpm.respuesta,                      IF(_xlpm.condicionesBeber,"Vendemos",_xlpm.respuestaEntrada),
+_xlpm.respuesta)</f>
+        <v>SinAlchohol</v>
+      </c>
+      <c r="G13" s="2" t="str">
+        <f t="shared" ref="G13:G14" si="8">IF(
+OR(F13="SinAlchohol",F13="EntradaNormal"),
+"Bienvenido",
+"Lo sentimos no puede pasar")</f>
+        <v>Bienvenido</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="str">
+        <f t="shared" ref="A14:C15" si="9">A5</f>
+        <v>Billy</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="C14" s="7" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Vendemos</v>
+      </c>
+      <c r="E14" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>Vendemos</v>
+      </c>
+      <c r="F14" s="9" t="str">
+        <f>_xlfn.LET(
+_xlpm.edadCliente,                 B14,
+_xlpm.edadAlchohol,             25,
+_xlpm.problemasAlcohol,    C14,
+_xlpm.edadEntrada,                18,
+_xlpm.edadConsumo,            _xlpm.edadCliente &gt;= _xlpm.edadAlchohol,
+_xlpm.puedeBeber,                NOT(_xlpm.problemasAlcohol),
+_xlpm.condicionesBeber,     AND(_xlpm.edadConsumo,_xlpm.puedeBeber),
+_xlpm.permisoEntrada,          _xlpm.edadCliente &gt;=  _xlpm.edadEntrada,
+_xlpm.respuestaEntrada,       IF(_xlpm.permisoEntrada,"SinAlchohol","NoPasar"),
 _xlpm.respuesta,                      IF(_xlpm.condicionesBeber,"EntradaNormal",_xlpm.respuestaEntrada),
 _xlpm.respuesta)</f>
         <v>EntradaNormal</v>
       </c>
-      <c r="G12" s="4" t="str">
+      <c r="G14" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Bienvenido</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>Bienvenido</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <f t="shared" si="10"/>
         <v>Marta</v>
       </c>
-      <c r="B13" s="4">
-        <f t="shared" si="10"/>
+      <c r="B15" s="2">
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="C13" s="9" t="b">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="7" t="str">
+      <c r="C15" s="7" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>NoVendemos</v>
+      </c>
+      <c r="E15" s="9" t="str">
         <f t="shared" si="6"/>
         <v>NoVendemos</v>
       </c>
-      <c r="E13" s="11" t="str">
+      <c r="F15" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>NoVendemos</v>
-      </c>
-      <c r="F13" s="11" t="str">
-        <f t="shared" si="8"/>
         <v>NoPasar</v>
       </c>
-      <c r="G13" s="4" t="str">
+      <c r="G15" s="2" t="str">
         <f>IF(
-OR(F13="SinAlchohol",F13="EntradaNormal"),
+OR(F15="SinAlchohol",F15="EntradaNormal"),
 "Bienvenido",
 "Vuelva a los 18")</f>
         <v>Vuelva a los 18</v>

</xml_diff>